<commit_message>
set codinghack30's recovery email
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="262">
   <si>
     <t>No</t>
   </si>
@@ -659,6 +659,9 @@
     <t>vpn</t>
   </si>
   <si>
+    <t>champion10875@gmail.com</t>
+  </si>
+  <si>
     <t>codinghack30</t>
   </si>
   <si>
@@ -731,12 +734,12 @@
     <t>golden_0810</t>
   </si>
   <si>
+    <t>goldenworrier1998</t>
+  </si>
+  <si>
     <t>onlyhi98</t>
   </si>
   <si>
-    <t>goldenworrier1998</t>
-  </si>
-  <si>
     <t>oogasuzuki@gmail.com</t>
   </si>
   <si>
@@ -750,6 +753,9 @@
   </si>
   <si>
     <t>high_92583</t>
+  </si>
+  <si>
+    <t>oogasuzuki</t>
   </si>
   <si>
     <t>nilsmikkola@gmail.com</t>
@@ -1728,7 +1734,9 @@
       <c r="J12" s="16"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="16"/>
+      <c r="A13" s="16" t="s">
+        <v>213</v>
+      </c>
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
       <c r="D13" s="37" t="s">
@@ -1736,19 +1744,19 @@
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="29" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G13" s="29" t="s">
         <v>188</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="I13" s="31" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
@@ -1759,20 +1767,20 @@
         <v>195</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="31" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="J14" s="31" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
@@ -1784,10 +1792,10 @@
       </c>
       <c r="E15" s="18"/>
       <c r="F15" s="29" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G15" s="42" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
@@ -1807,23 +1815,23 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="39" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="37" t="s">
         <v>185</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F17" s="29" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G17" s="42" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -1840,10 +1848,10 @@
       </c>
       <c r="E18" s="18"/>
       <c r="F18" s="29" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G18" s="42" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
@@ -1867,7 +1875,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="16" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
@@ -1876,10 +1884,10 @@
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="29" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G20" s="42" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
@@ -1899,22 +1907,24 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="39" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C22" s="29"/>
       <c r="D22" s="37" t="s">
         <v>185</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="G22" s="18"/>
+        <v>236</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>188</v>
+      </c>
       <c r="H22" s="29"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
@@ -1932,9 +1942,11 @@
         <v>192</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="G23" s="42"/>
+        <v>237</v>
+      </c>
+      <c r="G23" s="42" t="s">
+        <v>238</v>
+      </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
@@ -1962,7 +1974,7 @@
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="29" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="G25" s="42" t="s">
         <v>238</v>
@@ -1985,29 +1997,31 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="39" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="37" t="s">
         <v>185</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>242</v>
-      </c>
-      <c r="G27" s="18"/>
+        <v>243</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>188</v>
+      </c>
       <c r="H27" s="18"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="40" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
@@ -2018,9 +2032,11 @@
         <v>192</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="G28" s="18"/>
+        <v>244</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>245</v>
+      </c>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
@@ -2067,10 +2083,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="39" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C32" s="29"/>
       <c r="D32" s="37" t="s">
@@ -2096,10 +2112,10 @@
         <v>192</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="H33" s="18"/>
       <c r="I33" s="18"/>
@@ -2147,10 +2163,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="46" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C37" s="29"/>
       <c r="D37" s="29" t="s">
@@ -2177,13 +2193,13 @@
         <v>191</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
@@ -2239,7 +2255,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="40" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B42" s="29"/>
       <c r="C42" s="29"/>
@@ -2255,13 +2271,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="16" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D43" s="40">
         <v>12172085625</v>
@@ -2275,7 +2291,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="40" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B44" s="48" t="s">
         <v>192</v>
@@ -2284,7 +2300,7 @@
         <v>192</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
@@ -2295,12 +2311,12 @@
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="16" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B45" s="29"/>
       <c r="C45" s="29"/>
       <c r="D45" s="29" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
@@ -2311,7 +2327,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="40" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B46" s="48" t="s">
         <v>192</v>
@@ -2320,7 +2336,7 @@
         <v>192</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>

</xml_diff>

<commit_message>
change leekaifeng6's app pwd
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11850"/>
+    <workbookView windowWidth="21255" windowHeight="7410"/>
   </bookViews>
   <sheets>
     <sheet name="gmail" sheetId="1" r:id="rId1"/>
@@ -198,7 +198,7 @@
     <t>soft_0220</t>
   </si>
   <si>
-    <t>elez vftd iyzj mwcx</t>
+    <t>zpknksqmpndgrnul</t>
   </si>
   <si>
     <t>onlyhi6</t>
@@ -830,7 +830,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -893,13 +893,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -1046,7 +1039,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1086,12 +1079,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1466,70 +1453,73 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1541,73 +1531,70 @@
     <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2097,8 +2084,8 @@
   </sheetPr>
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2439,7 +2426,7 @@
       </c>
     </row>
     <row r="19" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A19" s="18">
+      <c r="A19" s="30">
         <v>12029671695</v>
       </c>
       <c r="B19" s="30"/>
@@ -2450,7 +2437,7 @@
       <c r="G19" s="40"/>
     </row>
     <row r="20" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="30" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="30"/>

</xml_diff>